<commit_message>
+ bổ sung Đăng ký _Doanh nghiệp
</commit_message>
<xml_diff>
--- a/Bao Cao Lien Tuc/Test_Error.xlsx
+++ b/Bao Cao Lien Tuc/Test_Error.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Test Validation" sheetId="1" r:id="rId1"/>
     <sheet name="Chức năng" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Giao diện" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="52">
   <si>
     <t>STT</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t xml:space="preserve">Trang chủ </t>
-  </si>
-  <si>
-    <t>_ Không kiểm tra độ dài các thông tin như mật khẩu, mật khẩu thanh toán, cmnd</t>
   </si>
   <si>
     <t xml:space="preserve">_Chưa bắt </t>
@@ -167,6 +164,17 @@
   <si>
     <t>Server Error in '/' Application.
 Cannot redirect after HTTP headers have been sent.</t>
+  </si>
+  <si>
+    <t>_ Phần nhập thông tin đăng nhập thấy ko hợp lý -&gt; chỉnh lại để ko bị bể</t>
+  </si>
+  <si>
+    <t>_Đăng ký _ Doanh nghiệp bị bể layout -&gt; nhảy và không đều</t>
+  </si>
+  <si>
+    <t>_ Chưa bắt validation cho trang Đăng ký doanh nghiệp
+_ Không kiểm tra độ dài các thông tin như mật khẩu, mật khẩu thanh toán, cmnd
+_ Chưa kiểm tra và bắt lỗi</t>
   </si>
 </sst>
 </file>
@@ -729,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:H89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F9:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -780,7 +788,7 @@
       <c r="G6" s="24"/>
       <c r="H6" s="25"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B7" s="22"/>
       <c r="C7" s="24">
         <v>2</v>
@@ -792,7 +800,7 @@
         <v>43</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G7" s="27"/>
       <c r="H7" s="25"/>
@@ -809,7 +817,7 @@
         <v>38</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="25"/>
@@ -1655,8 +1663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,10 +1706,10 @@
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="19" t="s">
         <v>48</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>49</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -2565,12 +2573,914 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B5:H89"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="72.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="20"/>
+      <c r="C5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="19"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="20"/>
+      <c r="C7" s="18">
+        <v>2</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="19"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="20"/>
+      <c r="C8" s="18">
+        <v>3</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="20"/>
+      <c r="C9" s="18">
+        <v>4</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="20"/>
+      <c r="C10" s="18">
+        <v>5</v>
+      </c>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="20"/>
+      <c r="C11" s="18">
+        <v>6</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="20"/>
+      <c r="C12" s="18">
+        <v>7</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="20"/>
+      <c r="C13" s="18">
+        <v>8</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="20"/>
+      <c r="C14" s="18">
+        <v>9</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="1">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="1">
+        <v>4</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="1">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C41" s="6"/>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C49" s="7"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="2">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C50" s="3"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="2">
+        <v>2</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C51" s="3"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="2">
+        <v>3</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C52" s="3"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="2">
+        <v>4</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C53" s="3"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="2">
+        <v>5</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G53" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C54" s="3"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="2">
+        <v>6</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C55" s="3"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="2">
+        <v>7</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C56" s="3"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="2">
+        <v>8</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C57" s="3"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="2">
+        <v>9</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C58" s="3"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="15">
+        <v>10</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C59" s="3"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="15">
+        <v>11</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C60" s="3"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="5">
+        <v>12</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C61" s="9"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="5">
+        <v>13</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H61" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C62" s="1">
+        <v>2</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+    </row>
+    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C63" s="3"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="1">
+        <v>1</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C64" s="3"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="1">
+        <v>2</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C65" s="3"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="1">
+        <v>3</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C66" s="3"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="1">
+        <v>4</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C67" s="1">
+        <v>3</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C68" s="7"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="2">
+        <v>1</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H68" s="1"/>
+    </row>
+    <row r="69" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C69" s="3"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="2">
+        <v>2</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H69" s="1"/>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C70" s="3"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="2">
+        <v>3</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H70" s="1"/>
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C71" s="3"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="2">
+        <v>4</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H71" s="1"/>
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C72" s="3"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="2">
+        <v>5</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C73" s="3"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="2">
+        <v>6</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="74" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C74" s="3"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="2">
+        <v>7</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C75" s="3"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="2">
+        <v>8</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H75" s="1"/>
+    </row>
+    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C76" s="3"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="2">
+        <v>9</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="77" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C77" s="3"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="15">
+        <v>10</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="78" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C78" s="9"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="15">
+        <v>11</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C79" s="1">
+        <v>4</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="80" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C80" s="3"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="1">
+        <v>1</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="81" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C81" s="3"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="82" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C82" s="3"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+    </row>
+    <row r="83" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C83" s="3"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+    </row>
+    <row r="84" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C84" s="3"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="11"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+    </row>
+    <row r="85" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C85" s="3"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+    </row>
+    <row r="86" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C86" s="3"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+    </row>
+    <row r="87" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C87" s="3"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="11"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+    </row>
+    <row r="88" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C88" s="3"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="11"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+    </row>
+    <row r="89" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C89" s="9"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>